<commit_message>
Possibly ready for alpha
Need to do some more validation, but runs and results appear reasonable. Need to validate results and do some checking, but committing what may be the final alpha code if checks are good.
</commit_message>
<xml_diff>
--- a/Health_Monte_Carlo_Input.xlsx
+++ b/Health_Monte_Carlo_Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beau/Git/Health_Insurance_Sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC11223-7FD0-4F43-907D-E873C9CCB3E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C7F061-6DF4-FD44-B306-D2F47E3CCB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{F6F7CCB2-3530-C445-A614-1A88D2B30731}"/>
   </bookViews>
@@ -302,7 +302,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Issue</t>
   </si>
@@ -440,6 +440,9 @@
   </si>
   <si>
     <t>Total w/ Premium</t>
+  </si>
+  <si>
+    <t>Output Mean</t>
   </si>
 </sst>
 </file>
@@ -1001,7 +1004,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B17" sqref="B17"/>
+      <selection pane="topRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1912,19 +1915,19 @@
         <v>33</v>
       </c>
       <c r="G25">
-        <v>15364</v>
+        <v>15976</v>
       </c>
       <c r="H25">
-        <v>17996</v>
+        <v>18056</v>
       </c>
       <c r="I25" s="12">
-        <v>17871</v>
+        <v>17906</v>
       </c>
       <c r="J25">
-        <v>12562</v>
+        <v>12512</v>
       </c>
       <c r="L25">
-        <v>16326</v>
+        <v>18407</v>
       </c>
       <c r="M25">
         <v>24223</v>
@@ -1943,23 +1946,23 @@
       </c>
       <c r="G26" s="25">
         <f>G24-G25</f>
-        <v>-88</v>
+        <v>-700</v>
       </c>
       <c r="H26" s="25">
         <f>H24-H25</f>
-        <v>0</v>
+        <v>-60</v>
       </c>
       <c r="I26" s="25">
         <f>I24-I25</f>
-        <v>-15</v>
+        <v>-50</v>
       </c>
       <c r="J26" s="25">
         <f>J24-J25</f>
-        <v>-250</v>
+        <v>-200</v>
       </c>
       <c r="L26" s="25">
         <f>L24-L25</f>
-        <v>1831.8239999999969</v>
+        <v>-249.17600000000311</v>
       </c>
       <c r="M26" s="25">
         <f>M24-M25</f>
@@ -2277,9 +2280,62 @@
       <c r="P34" s="12"/>
     </row>
     <row r="35" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F35" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G35">
+        <v>15203</v>
+      </c>
+      <c r="H35">
+        <v>13221</v>
+      </c>
+      <c r="I35" s="12">
+        <v>14180</v>
+      </c>
+      <c r="J35">
+        <v>12318</v>
+      </c>
+      <c r="L35">
+        <v>17567</v>
+      </c>
       <c r="P35" s="22"/>
     </row>
     <row r="36" spans="6:16" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" s="25">
+        <f>G34-G35</f>
+        <v>73</v>
+      </c>
+      <c r="H36" s="25">
+        <f>H34-H35</f>
+        <v>4860</v>
+      </c>
+      <c r="I36" s="25">
+        <f>I34-I35</f>
+        <v>4243</v>
+      </c>
+      <c r="J36" s="25">
+        <f>J34-J35</f>
+        <v>5411</v>
+      </c>
+      <c r="L36" s="25">
+        <f>L34-L35</f>
+        <v>1539.8239999999969</v>
+      </c>
+      <c r="M36" s="25">
+        <f>M34-M35</f>
+        <v>20959.362666666668</v>
+      </c>
+      <c r="N36" s="25">
+        <f>N34-N35</f>
+        <v>23761.847999999998</v>
+      </c>
+      <c r="O36" s="25">
+        <f>O34-O35</f>
+        <v>17961.988000000001</v>
+      </c>
       <c r="P36" s="21"/>
     </row>
     <row r="37" spans="6:16" x14ac:dyDescent="0.2">

</xml_diff>